<commit_message>
Conflict Fix and Penalty scaling to 0 to 100%
Fixed the conflict, and scaled the penalty to match scale of 0 to 100%.
</commit_message>
<xml_diff>
--- a/output/main/Optimization_Stats.xlsx
+++ b/output/main/Optimization_Stats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
   <si>
     <t>Schedule (Pre-Optimization)</t>
   </si>
@@ -107,34 +107,28 @@
     <t>Schedule (Post-Optimization)</t>
   </si>
   <si>
-    <t>84.09%</t>
+    <t>86.36%</t>
   </si>
   <si>
     <t>77.27%</t>
   </si>
   <si>
-    <t>86.36%</t>
-  </si>
-  <si>
-    <t>87.5%</t>
+    <t>88.64%</t>
   </si>
   <si>
     <t>100.0%</t>
   </si>
   <si>
-    <t>45.45%</t>
-  </si>
-  <si>
-    <t>69.7%</t>
-  </si>
-  <si>
-    <t>84.85%</t>
+    <t>50.0%</t>
+  </si>
+  <si>
+    <t>68.94%</t>
   </si>
   <si>
     <t>Optimization Time</t>
   </si>
   <si>
-    <t>3 min, 22 sec</t>
+    <t>2 min, 59 sec</t>
   </si>
 </sst>
 </file>
@@ -677,19 +671,19 @@
         <v>44.0</v>
       </c>
       <c r="C16" t="n" s="1">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
       <c r="D16" t="n" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="E16" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="F16" t="n" s="1">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="G16" t="s" s="1">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H16" t="s" s="1">
         <v>31</v>
@@ -701,7 +695,7 @@
         <v>9.0</v>
       </c>
       <c r="K16" t="n" s="1">
-        <v>106.36</v>
+        <v>92.55</v>
       </c>
     </row>
     <row r="17">
@@ -736,7 +730,7 @@
         <v>9.0</v>
       </c>
       <c r="K17" t="n" s="1">
-        <v>118.18</v>
+        <v>120.18</v>
       </c>
     </row>
     <row r="18">
@@ -747,10 +741,10 @@
         <v>88.0</v>
       </c>
       <c r="C18" t="n" s="1">
-        <v>77.0</v>
+        <v>78.0</v>
       </c>
       <c r="D18" t="n" s="1">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="E18" t="n" s="1">
         <v>88.0</v>
@@ -759,10 +753,10 @@
         <v>12.0</v>
       </c>
       <c r="G18" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="H18" t="s" s="1">
         <v>33</v>
-      </c>
-      <c r="H18" t="s" s="1">
-        <v>34</v>
       </c>
       <c r="I18" t="n" s="1">
         <v>8.0</v>
@@ -771,7 +765,7 @@
         <v>9.0</v>
       </c>
       <c r="K18" t="n" s="1">
-        <v>109.91</v>
+        <v>101.91</v>
       </c>
     </row>
     <row r="19">
@@ -797,7 +791,7 @@
         <v>25</v>
       </c>
       <c r="H19" t="s" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I19" t="n" s="1">
         <v>3.0</v>
@@ -826,13 +820,13 @@
         <v>22.0</v>
       </c>
       <c r="F20" t="n" s="1">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="G20" t="s" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20" t="s" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I20" t="n" s="1">
         <v>3.0</v>
@@ -841,7 +835,7 @@
         <v>7.0</v>
       </c>
       <c r="K20" t="n" s="1">
-        <v>170.64</v>
+        <v>157.0</v>
       </c>
     </row>
     <row r="21">
@@ -861,13 +855,13 @@
         <v>44.0</v>
       </c>
       <c r="F21" t="n" s="1">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="G21" t="s" s="1">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="H21" t="s" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I21" t="n" s="1">
         <v>5.0</v>
@@ -876,7 +870,7 @@
         <v>8.0</v>
       </c>
       <c r="K21" t="n" s="1">
-        <v>79.55</v>
+        <v>93.18</v>
       </c>
     </row>
     <row r="22">
@@ -902,7 +896,7 @@
         <v>15</v>
       </c>
       <c r="H22" t="s" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I22" t="n" s="1">
         <v>5.0</v>
@@ -946,7 +940,7 @@
         <v>9.0</v>
       </c>
       <c r="K23" t="n" s="1">
-        <v>105.82</v>
+        <v>107.82</v>
       </c>
     </row>
     <row r="24">
@@ -966,13 +960,13 @@
         <v>44.0</v>
       </c>
       <c r="F24" t="n" s="1">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="G24" t="s" s="1">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H24" t="s" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I24" t="n" s="1">
         <v>5.0</v>
@@ -981,7 +975,7 @@
         <v>8.0</v>
       </c>
       <c r="K24" t="n" s="1">
-        <v>106.82</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="25">
@@ -992,22 +986,22 @@
         <v>44.0</v>
       </c>
       <c r="C25" t="n" s="1">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="D25" t="n" s="1">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="E25" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="F25" t="n" s="1">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="G25" t="s" s="1">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H25" t="s" s="1">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I25" t="n" s="1">
         <v>4.0</v>
@@ -1016,7 +1010,7 @@
         <v>9.0</v>
       </c>
       <c r="K25" t="n" s="1">
-        <v>118.0</v>
+        <v>113.36</v>
       </c>
     </row>
     <row r="26">
@@ -1027,22 +1021,22 @@
         <v>132.0</v>
       </c>
       <c r="C26" t="n" s="1">
-        <v>112.0</v>
+        <v>114.0</v>
       </c>
       <c r="D26" t="n" s="1">
-        <v>20.0</v>
+        <v>18.0</v>
       </c>
       <c r="E26" t="n" s="1">
         <v>132.0</v>
       </c>
       <c r="F26" t="n" s="1">
-        <v>40.0</v>
+        <v>41.0</v>
       </c>
       <c r="G26" t="s" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H26" t="s" s="1">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I26" t="n" s="1">
         <v>12.0</v>
@@ -1051,17 +1045,17 @@
         <v>9.0</v>
       </c>
       <c r="K26" t="n" s="1">
-        <v>223.91</v>
+        <v>209.18</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug for RestDay penalization
</commit_message>
<xml_diff>
--- a/output/main/Optimization_Stats.xlsx
+++ b/output/main/Optimization_Stats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
   <si>
     <t>Schedule (Pre-Optimization)</t>
   </si>
@@ -50,6 +50,9 @@
     <t>Division U7 (Tier: 1)</t>
   </si>
   <si>
+    <t>77.27%</t>
+  </si>
+  <si>
     <t>75.0%</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
     <t>Division U7 (Tier: 3)</t>
   </si>
   <si>
+    <t>85.23%</t>
+  </si>
+  <si>
     <t>81.82%</t>
   </si>
   <si>
@@ -77,6 +83,9 @@
     <t>Division U8 (Tier: 2)</t>
   </si>
   <si>
+    <t>65.91%</t>
+  </si>
+  <si>
     <t>63.64%</t>
   </si>
   <si>
@@ -101,34 +110,43 @@
     <t>Division U9 (Tier: 3)</t>
   </si>
   <si>
+    <t>69.7%</t>
+  </si>
+  <si>
     <t>67.42%</t>
   </si>
   <si>
     <t>Schedule (Post-Optimization)</t>
   </si>
   <si>
-    <t>86.36%</t>
-  </si>
-  <si>
-    <t>77.27%</t>
-  </si>
-  <si>
-    <t>88.64%</t>
+    <t>95.45%</t>
+  </si>
+  <si>
+    <t>93.18%</t>
+  </si>
+  <si>
+    <t>71.59%</t>
   </si>
   <si>
     <t>100.0%</t>
   </si>
   <si>
-    <t>50.0%</t>
-  </si>
-  <si>
-    <t>68.94%</t>
+    <t>54.55%</t>
+  </si>
+  <si>
+    <t>90.91%</t>
+  </si>
+  <si>
+    <t>70.45%</t>
+  </si>
+  <si>
+    <t>60.61%</t>
   </si>
   <si>
     <t>Optimization Time</t>
   </si>
   <si>
-    <t>2 min, 59 sec</t>
+    <t>2 min, 13 sec</t>
   </si>
 </sst>
 </file>
@@ -260,13 +278,13 @@
         <v>44.0</v>
       </c>
       <c r="F2" t="n" s="1">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="G2" t="s" s="1">
         <v>12</v>
       </c>
       <c r="H2" t="s" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" t="n" s="1">
         <v>4.0</v>
@@ -275,12 +293,12 @@
         <v>8.0</v>
       </c>
       <c r="K2" t="n" s="1">
-        <v>146.0</v>
+        <v>205.86</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="n" s="1">
         <v>44.0</v>
@@ -298,10 +316,10 @@
         <v>11.0</v>
       </c>
       <c r="G3" t="s" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I3" t="n" s="1">
         <v>4.0</v>
@@ -310,12 +328,12 @@
         <v>8.0</v>
       </c>
       <c r="K3" t="n" s="1">
-        <v>144.0</v>
+        <v>221.82</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="n" s="1">
         <v>88.0</v>
@@ -330,13 +348,13 @@
         <v>88.0</v>
       </c>
       <c r="F4" t="n" s="1">
-        <v>16.0</v>
+        <v>13.0</v>
       </c>
       <c r="G4" t="s" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I4" t="n" s="1">
         <v>8.0</v>
@@ -345,12 +363,12 @@
         <v>9.0</v>
       </c>
       <c r="K4" t="n" s="1">
-        <v>157.55</v>
+        <v>212.33999999999997</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" t="n" s="1">
         <v>22.0</v>
@@ -368,10 +386,10 @@
         <v>7.0</v>
       </c>
       <c r="G5" t="s" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I5" t="n" s="1">
         <v>3.0</v>
@@ -380,12 +398,12 @@
         <v>5.0</v>
       </c>
       <c r="K5" t="n" s="1">
-        <v>134.45</v>
+        <v>334.45</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" t="n" s="1">
         <v>22.0</v>
@@ -403,10 +421,10 @@
         <v>13.0</v>
       </c>
       <c r="G6" t="s" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I6" t="n" s="1">
         <v>3.0</v>
@@ -415,12 +433,12 @@
         <v>3.0</v>
       </c>
       <c r="K6" t="n" s="1">
-        <v>255.27</v>
+        <v>386.99</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" t="n" s="1">
         <v>44.0</v>
@@ -435,13 +453,13 @@
         <v>44.0</v>
       </c>
       <c r="F7" t="n" s="1">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="G7" t="s" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s" s="1">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I7" t="n" s="1">
         <v>5.0</v>
@@ -450,12 +468,12 @@
         <v>5.0</v>
       </c>
       <c r="K7" t="n" s="1">
-        <v>193.09</v>
+        <v>291.37</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B8" t="n" s="1">
         <v>44.0</v>
@@ -470,13 +488,13 @@
         <v>44.0</v>
       </c>
       <c r="F8" t="n" s="1">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="G8" t="s" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s" s="1">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I8" t="n" s="1">
         <v>5.0</v>
@@ -485,12 +503,12 @@
         <v>7.0</v>
       </c>
       <c r="K8" t="n" s="1">
-        <v>102.36</v>
+        <v>175.26999999999998</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B9" t="n" s="1">
         <v>22.0</v>
@@ -508,10 +526,10 @@
         <v>6.0</v>
       </c>
       <c r="G9" t="s" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H9" t="s" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I9" t="n" s="1">
         <v>2.0</v>
@@ -520,12 +538,12 @@
         <v>8.0</v>
       </c>
       <c r="K9" t="n" s="1">
-        <v>119.82</v>
+        <v>181.43</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" t="n" s="1">
         <v>44.0</v>
@@ -540,13 +558,13 @@
         <v>44.0</v>
       </c>
       <c r="F10" t="n" s="1">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="G10" t="s" s="1">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I10" t="n" s="1">
         <v>5.0</v>
@@ -555,12 +573,12 @@
         <v>6.0</v>
       </c>
       <c r="K10" t="n" s="1">
-        <v>134.82</v>
+        <v>203.73000000000002</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" t="n" s="1">
         <v>44.0</v>
@@ -578,10 +596,10 @@
         <v>12.0</v>
       </c>
       <c r="G11" t="s" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H11" t="s" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I11" t="n" s="1">
         <v>4.0</v>
@@ -590,12 +608,12 @@
         <v>8.0</v>
       </c>
       <c r="K11" t="n" s="1">
-        <v>158.82</v>
+        <v>230.19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B12" t="n" s="1">
         <v>132.0</v>
@@ -610,13 +628,13 @@
         <v>132.0</v>
       </c>
       <c r="F12" t="n" s="1">
-        <v>43.0</v>
+        <v>40.0</v>
       </c>
       <c r="G12" t="s" s="1">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s" s="1">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I12" t="n" s="1">
         <v>12.0</v>
@@ -625,12 +643,12 @@
         <v>7.0</v>
       </c>
       <c r="K12" t="n" s="1">
-        <v>374.73</v>
+        <v>435.58</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s" s="2">
         <v>1</v>
@@ -671,106 +689,106 @@
         <v>44.0</v>
       </c>
       <c r="C16" t="n" s="1">
-        <v>38.0</v>
+        <v>42.0</v>
       </c>
       <c r="D16" t="n" s="1">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="E16" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="F16" t="n" s="1">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="G16" t="s" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s" s="1">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I16" t="n" s="1">
         <v>4.0</v>
       </c>
       <c r="J16" t="n" s="1">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="K16" t="n" s="1">
-        <v>92.55</v>
+        <v>134.66</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="C17" t="n" s="1">
-        <v>36.0</v>
+        <v>41.0</v>
       </c>
       <c r="D17" t="n" s="1">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="E17" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="F17" t="n" s="1">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="G17" t="s" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H17" t="s" s="1">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="I17" t="n" s="1">
         <v>4.0</v>
       </c>
       <c r="J17" t="n" s="1">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="K17" t="n" s="1">
-        <v>120.18</v>
+        <v>152.03</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" t="n" s="1">
         <v>88.0</v>
       </c>
       <c r="C18" t="n" s="1">
-        <v>78.0</v>
+        <v>82.0</v>
       </c>
       <c r="D18" t="n" s="1">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="E18" t="n" s="1">
         <v>88.0</v>
       </c>
       <c r="F18" t="n" s="1">
-        <v>12.0</v>
+        <v>25.0</v>
       </c>
       <c r="G18" t="s" s="1">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H18" t="s" s="1">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I18" t="n" s="1">
         <v>8.0</v>
       </c>
       <c r="J18" t="n" s="1">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="K18" t="n" s="1">
-        <v>101.91</v>
+        <v>176.05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" t="n" s="1">
         <v>22.0</v>
@@ -785,13 +803,13 @@
         <v>22.0</v>
       </c>
       <c r="F19" t="n" s="1">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="G19" t="s" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H19" t="s" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I19" t="n" s="1">
         <v>3.0</v>
@@ -800,12 +818,12 @@
         <v>7.0</v>
       </c>
       <c r="K19" t="n" s="1">
-        <v>88.82</v>
+        <v>177.37</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" t="n" s="1">
         <v>22.0</v>
@@ -820,13 +838,13 @@
         <v>22.0</v>
       </c>
       <c r="F20" t="n" s="1">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="G20" t="s" s="1">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H20" t="s" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I20" t="n" s="1">
         <v>3.0</v>
@@ -835,12 +853,12 @@
         <v>7.0</v>
       </c>
       <c r="K20" t="n" s="1">
-        <v>157.0</v>
+        <v>225.81</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21" t="n" s="1">
         <v>44.0</v>
@@ -855,13 +873,13 @@
         <v>44.0</v>
       </c>
       <c r="F21" t="n" s="1">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="G21" t="s" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H21" t="s" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I21" t="n" s="1">
         <v>5.0</v>
@@ -870,12 +888,12 @@
         <v>8.0</v>
       </c>
       <c r="K21" t="n" s="1">
-        <v>93.18</v>
+        <v>167.01999999999998</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B22" t="n" s="1">
         <v>44.0</v>
@@ -890,13 +908,13 @@
         <v>44.0</v>
       </c>
       <c r="F22" t="n" s="1">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="G22" t="s" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H22" t="s" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I22" t="n" s="1">
         <v>5.0</v>
@@ -905,21 +923,21 @@
         <v>8.0</v>
       </c>
       <c r="K22" t="n" s="1">
-        <v>79.55</v>
+        <v>149.96</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B23" t="n" s="1">
         <v>22.0</v>
       </c>
       <c r="C23" t="n" s="1">
-        <v>18.0</v>
+        <v>20.0</v>
       </c>
       <c r="D23" t="n" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="E23" t="n" s="1">
         <v>22.0</v>
@@ -928,24 +946,24 @@
         <v>6.0</v>
       </c>
       <c r="G23" t="s" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H23" t="s" s="1">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I23" t="n" s="1">
         <v>2.0</v>
       </c>
       <c r="J23" t="n" s="1">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="K23" t="n" s="1">
-        <v>107.82</v>
+        <v>131.89999999999998</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n" s="1">
         <v>44.0</v>
@@ -960,13 +978,13 @@
         <v>44.0</v>
       </c>
       <c r="F24" t="n" s="1">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="G24" t="s" s="1">
         <v>12</v>
       </c>
       <c r="H24" t="s" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I24" t="n" s="1">
         <v>5.0</v>
@@ -975,87 +993,87 @@
         <v>8.0</v>
       </c>
       <c r="K24" t="n" s="1">
-        <v>100.0</v>
+        <v>155.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B25" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="C25" t="n" s="1">
-        <v>36.0</v>
+        <v>41.0</v>
       </c>
       <c r="D25" t="n" s="1">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="E25" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="F25" t="n" s="1">
-        <v>9.0</v>
+        <v>13.0</v>
       </c>
       <c r="G25" t="s" s="1">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="H25" t="s" s="1">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="I25" t="n" s="1">
         <v>4.0</v>
       </c>
       <c r="J25" t="n" s="1">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="K25" t="n" s="1">
-        <v>113.36</v>
+        <v>172.26999999999998</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B26" t="n" s="1">
         <v>132.0</v>
       </c>
       <c r="C26" t="n" s="1">
-        <v>114.0</v>
+        <v>123.0</v>
       </c>
       <c r="D26" t="n" s="1">
-        <v>18.0</v>
+        <v>9.0</v>
       </c>
       <c r="E26" t="n" s="1">
         <v>132.0</v>
       </c>
       <c r="F26" t="n" s="1">
-        <v>41.0</v>
+        <v>52.0</v>
       </c>
       <c r="G26" t="s" s="1">
+        <v>42</v>
+      </c>
+      <c r="H26" t="s" s="1">
         <v>36</v>
-      </c>
-      <c r="H26" t="s" s="1">
-        <v>31</v>
       </c>
       <c r="I26" t="n" s="1">
         <v>12.0</v>
       </c>
       <c r="J26" t="n" s="1">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="K26" t="n" s="1">
-        <v>209.18</v>
+        <v>230.3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Temporary Fix for RestDayEquality Penalty Value: - Separated exhibition games from list of total games and only iterates through non-exhibition games when calculating penalty
Signed-off-by: Brady Norton <bnort.11@gmail.com>
</commit_message>
<xml_diff>
--- a/output/main/Optimization_Stats.xlsx
+++ b/output/main/Optimization_Stats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Schedule (Pre-Optimization)</t>
   </si>
@@ -44,7 +44,7 @@
     <t>Games per Team</t>
   </si>
   <si>
-    <t>Quality</t>
+    <t>Penalty</t>
   </si>
   <si>
     <t>Division U7 (Tier: 1)</t>
@@ -59,10 +59,10 @@
     <t>Division U8 (Tier: 0)</t>
   </si>
   <si>
-    <t>90.34%</t>
-  </si>
-  <si>
-    <t>61.15%</t>
+    <t>90.91%</t>
+  </si>
+  <si>
+    <t>61.54%</t>
   </si>
   <si>
     <t>Division U9 (Tier: 0)</t>
@@ -77,19 +77,22 @@
     <t>Schedule (Post-Optimization)</t>
   </si>
   <si>
-    <t>87.67%</t>
+    <t>89.43%</t>
+  </si>
+  <si>
+    <t>91.48%</t>
   </si>
   <si>
     <t>78.85%</t>
   </si>
   <si>
-    <t>90.22%</t>
+    <t>89.13%</t>
   </si>
   <si>
     <t>Optimization Time</t>
   </si>
   <si>
-    <t>0 min, 30 sec</t>
+    <t>0 min, 11 sec</t>
   </si>
 </sst>
 </file>
@@ -106,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +124,46 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="9ECA80"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="9ECA80"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFEAAF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAAF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFD96D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD96D"/>
       </patternFill>
     </fill>
   </fills>
@@ -136,12 +179,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
   </cellXfs>
@@ -211,10 +266,10 @@
       <c r="B2" t="n" s="1">
         <v>227.0</v>
       </c>
-      <c r="C2" t="n" s="1">
+      <c r="C2" t="n" s="6">
         <v>164.0</v>
       </c>
-      <c r="D2" t="n" s="1">
+      <c r="D2" t="n" s="6">
         <v>63.0</v>
       </c>
       <c r="E2" t="n" s="1">
@@ -226,17 +281,17 @@
       <c r="G2" t="s" s="1">
         <v>12</v>
       </c>
-      <c r="H2" t="s" s="1">
+      <c r="H2" t="s" s="6">
         <v>13</v>
       </c>
       <c r="I2" t="n" s="1">
         <v>16.0</v>
       </c>
-      <c r="J2" t="n" s="1">
+      <c r="J2" t="n" s="5">
         <v>10.0</v>
       </c>
-      <c r="K2" t="n" s="1">
-        <v>514.45</v>
+      <c r="K2" t="n" s="6">
+        <v>509.45</v>
       </c>
     </row>
     <row r="3">
@@ -246,32 +301,32 @@
       <c r="B3" t="n" s="1">
         <v>260.0</v>
       </c>
-      <c r="C3" t="n" s="1">
-        <v>159.0</v>
-      </c>
-      <c r="D3" t="n" s="1">
-        <v>101.0</v>
+      <c r="C3" t="n" s="6">
+        <v>160.0</v>
+      </c>
+      <c r="D3" t="n" s="6">
+        <v>100.0</v>
       </c>
       <c r="E3" t="n" s="1">
         <v>176.0</v>
       </c>
-      <c r="F3" t="n" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="G3" t="s" s="1">
+      <c r="F3" t="n" s="5">
+        <v>16.0</v>
+      </c>
+      <c r="G3" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="H3" t="s" s="1">
+      <c r="H3" t="s" s="6">
         <v>16</v>
       </c>
       <c r="I3" t="n" s="1">
         <v>16.0</v>
       </c>
-      <c r="J3" t="n" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="K3" t="n" s="1">
-        <v>728.98</v>
+      <c r="J3" t="n" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="K3" t="n" s="6">
+        <v>709.27</v>
       </c>
     </row>
     <row r="4">
@@ -281,10 +336,10 @@
       <c r="B4" t="n" s="1">
         <v>276.0</v>
       </c>
-      <c r="C4" t="n" s="1">
+      <c r="C4" t="n" s="6">
         <v>205.0</v>
       </c>
-      <c r="D4" t="n" s="1">
+      <c r="D4" t="n" s="6">
         <v>71.0</v>
       </c>
       <c r="E4" t="n" s="1">
@@ -296,17 +351,17 @@
       <c r="G4" t="s" s="1">
         <v>18</v>
       </c>
-      <c r="H4" t="s" s="1">
+      <c r="H4" t="s" s="5">
         <v>19</v>
       </c>
       <c r="I4" t="n" s="1">
         <v>23.0</v>
       </c>
-      <c r="J4" t="n" s="1">
+      <c r="J4" t="n" s="5">
         <v>8.0</v>
       </c>
-      <c r="K4" t="n" s="1">
-        <v>884.87</v>
+      <c r="K4" t="n" s="6">
+        <v>851.87</v>
       </c>
     </row>
     <row r="15">
@@ -351,11 +406,11 @@
       <c r="B16" t="n" s="1">
         <v>227.0</v>
       </c>
-      <c r="C16" t="n" s="1">
-        <v>199.0</v>
-      </c>
-      <c r="D16" t="n" s="1">
-        <v>28.0</v>
+      <c r="C16" t="n" s="4">
+        <v>203.0</v>
+      </c>
+      <c r="D16" t="n" s="4">
+        <v>24.0</v>
       </c>
       <c r="E16" t="n" s="1">
         <v>176.0</v>
@@ -366,17 +421,17 @@
       <c r="G16" t="s" s="1">
         <v>12</v>
       </c>
-      <c r="H16" t="s" s="1">
+      <c r="H16" t="s" s="4">
         <v>21</v>
       </c>
       <c r="I16" t="n" s="1">
         <v>16.0</v>
       </c>
-      <c r="J16" t="n" s="1">
+      <c r="J16" t="n" s="3">
         <v>12.0</v>
       </c>
-      <c r="K16" t="n" s="1">
-        <v>326.45</v>
+      <c r="K16" t="n" s="4">
+        <v>307.45</v>
       </c>
     </row>
     <row r="17">
@@ -386,32 +441,32 @@
       <c r="B17" t="n" s="1">
         <v>260.0</v>
       </c>
-      <c r="C17" t="n" s="1">
+      <c r="C17" t="n" s="4">
         <v>205.0</v>
       </c>
-      <c r="D17" t="n" s="1">
+      <c r="D17" t="n" s="4">
         <v>55.0</v>
       </c>
       <c r="E17" t="n" s="1">
         <v>176.0</v>
       </c>
-      <c r="F17" t="n" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="G17" t="s" s="1">
-        <v>15</v>
-      </c>
-      <c r="H17" t="s" s="1">
+      <c r="F17" t="n" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="G17" t="s" s="3">
         <v>22</v>
+      </c>
+      <c r="H17" t="s" s="4">
+        <v>23</v>
       </c>
       <c r="I17" t="n" s="1">
         <v>16.0</v>
       </c>
-      <c r="J17" t="n" s="1">
+      <c r="J17" t="n" s="3">
         <v>12.0</v>
       </c>
-      <c r="K17" t="n" s="1">
-        <v>475.98</v>
+      <c r="K17" t="n" s="4">
+        <v>454.57</v>
       </c>
     </row>
     <row r="18">
@@ -421,11 +476,11 @@
       <c r="B18" t="n" s="1">
         <v>276.0</v>
       </c>
-      <c r="C18" t="n" s="1">
-        <v>249.0</v>
-      </c>
-      <c r="D18" t="n" s="1">
-        <v>27.0</v>
+      <c r="C18" t="n" s="4">
+        <v>246.0</v>
+      </c>
+      <c r="D18" t="n" s="4">
+        <v>30.0</v>
       </c>
       <c r="E18" t="n" s="1">
         <v>242.0</v>
@@ -436,27 +491,27 @@
       <c r="G18" t="s" s="1">
         <v>18</v>
       </c>
-      <c r="H18" t="s" s="1">
-        <v>23</v>
+      <c r="H18" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="I18" t="n" s="1">
         <v>23.0</v>
       </c>
-      <c r="J18" t="n" s="1">
+      <c r="J18" t="n" s="3">
         <v>10.0</v>
       </c>
-      <c r="K18" t="n" s="1">
-        <v>758.87</v>
+      <c r="K18" t="n" s="4">
+        <v>741.87</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added directory for Executable file - Outputs now located in MultivariableSportScheduler/Exe/output
Signed-off-by: Brady Norton <bnort.11@gmail.com>
</commit_message>
<xml_diff>
--- a/output/main/Optimization_Stats.xlsx
+++ b/output/main/Optimization_Stats.xlsx
@@ -68,22 +68,22 @@
     <t>Division U9 (Tier: 0)</t>
   </si>
   <si>
-    <t>84.71%</t>
-  </si>
-  <si>
-    <t>74.28%</t>
+    <t>84.3%</t>
+  </si>
+  <si>
+    <t>73.91%</t>
   </si>
   <si>
     <t>Schedule (Post-Optimization)</t>
   </si>
   <si>
-    <t>89.43%</t>
-  </si>
-  <si>
-    <t>91.48%</t>
-  </si>
-  <si>
-    <t>78.85%</t>
+    <t>93.75%</t>
+  </si>
+  <si>
+    <t>87.22%</t>
+  </si>
+  <si>
+    <t>81.92%</t>
   </si>
   <si>
     <t>89.13%</t>
@@ -92,7 +92,7 @@
     <t>Optimization Time</t>
   </si>
   <si>
-    <t>0 min, 11 sec</t>
+    <t>0 min, 10 sec</t>
   </si>
 </sst>
 </file>
@@ -275,13 +275,13 @@
       <c r="E2" t="n" s="1">
         <v>176.0</v>
       </c>
-      <c r="F2" t="n" s="1">
+      <c r="F2" t="n" s="5">
         <v>12.0</v>
       </c>
-      <c r="G2" t="s" s="1">
+      <c r="G2" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="H2" t="s" s="6">
+      <c r="H2" t="s" s="5">
         <v>13</v>
       </c>
       <c r="I2" t="n" s="1">
@@ -291,7 +291,7 @@
         <v>10.0</v>
       </c>
       <c r="K2" t="n" s="6">
-        <v>509.45</v>
+        <v>526.45</v>
       </c>
     </row>
     <row r="3">
@@ -310,10 +310,10 @@
       <c r="E3" t="n" s="1">
         <v>176.0</v>
       </c>
-      <c r="F3" t="n" s="5">
+      <c r="F3" t="n" s="1">
         <v>16.0</v>
       </c>
-      <c r="G3" t="s" s="5">
+      <c r="G3" t="s" s="1">
         <v>15</v>
       </c>
       <c r="H3" t="s" s="6">
@@ -326,7 +326,7 @@
         <v>10.0</v>
       </c>
       <c r="K3" t="n" s="6">
-        <v>709.27</v>
+        <v>725.27</v>
       </c>
     </row>
     <row r="4">
@@ -337,21 +337,21 @@
         <v>276.0</v>
       </c>
       <c r="C4" t="n" s="6">
-        <v>205.0</v>
+        <v>204.0</v>
       </c>
       <c r="D4" t="n" s="6">
-        <v>71.0</v>
+        <v>72.0</v>
       </c>
       <c r="E4" t="n" s="1">
         <v>242.0</v>
       </c>
       <c r="F4" t="n" s="1">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
       <c r="G4" t="s" s="1">
         <v>18</v>
       </c>
-      <c r="H4" t="s" s="5">
+      <c r="H4" t="s" s="6">
         <v>19</v>
       </c>
       <c r="I4" t="n" s="1">
@@ -361,7 +361,7 @@
         <v>8.0</v>
       </c>
       <c r="K4" t="n" s="6">
-        <v>851.87</v>
+        <v>834.11</v>
       </c>
     </row>
     <row r="15">
@@ -407,22 +407,22 @@
         <v>227.0</v>
       </c>
       <c r="C16" t="n" s="4">
-        <v>203.0</v>
+        <v>198.0</v>
       </c>
       <c r="D16" t="n" s="4">
-        <v>24.0</v>
+        <v>29.0</v>
       </c>
       <c r="E16" t="n" s="1">
         <v>176.0</v>
       </c>
-      <c r="F16" t="n" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="G16" t="s" s="1">
-        <v>12</v>
-      </c>
-      <c r="H16" t="s" s="4">
+      <c r="F16" t="n" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="G16" t="s" s="3">
         <v>21</v>
+      </c>
+      <c r="H16" t="s" s="3">
+        <v>22</v>
       </c>
       <c r="I16" t="n" s="1">
         <v>16.0</v>
@@ -431,7 +431,7 @@
         <v>12.0</v>
       </c>
       <c r="K16" t="n" s="4">
-        <v>307.45</v>
+        <v>324.75</v>
       </c>
     </row>
     <row r="17">
@@ -442,19 +442,19 @@
         <v>260.0</v>
       </c>
       <c r="C17" t="n" s="4">
-        <v>205.0</v>
+        <v>213.0</v>
       </c>
       <c r="D17" t="n" s="4">
-        <v>55.0</v>
+        <v>47.0</v>
       </c>
       <c r="E17" t="n" s="1">
         <v>176.0</v>
       </c>
-      <c r="F17" t="n" s="3">
-        <v>15.0</v>
-      </c>
-      <c r="G17" t="s" s="3">
-        <v>22</v>
+      <c r="F17" t="n" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="G17" t="s" s="1">
+        <v>15</v>
       </c>
       <c r="H17" t="s" s="4">
         <v>23</v>
@@ -463,10 +463,10 @@
         <v>16.0</v>
       </c>
       <c r="J17" t="n" s="3">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="K17" t="n" s="4">
-        <v>454.57</v>
+        <v>425.27</v>
       </c>
     </row>
     <row r="18">
@@ -486,12 +486,12 @@
         <v>242.0</v>
       </c>
       <c r="F18" t="n" s="1">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
       <c r="G18" t="s" s="1">
         <v>18</v>
       </c>
-      <c r="H18" t="s" s="3">
+      <c r="H18" t="s" s="4">
         <v>24</v>
       </c>
       <c r="I18" t="n" s="1">
@@ -501,7 +501,7 @@
         <v>10.0</v>
       </c>
       <c r="K18" t="n" s="4">
-        <v>741.87</v>
+        <v>736.11</v>
       </c>
     </row>
     <row r="29">

</xml_diff>